<commit_message>
Add printStackTrace to SonarQube report
</commit_message>
<xml_diff>
--- a/SonarQube/SonarQubeReport.xlsx
+++ b/SonarQube/SonarQubeReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETF\13M111RBS\rbs2023-2024\SonarQube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0658407-4345-4D44-A58D-6662FA59B1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCB5074-FEE6-4D23-B83D-BBBC01BFEB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="625">
   <si>
     <t>Rule</t>
   </si>
@@ -1825,6 +1825,84 @@
   </si>
   <si>
     <t>Brisanje iz tabele users pri brisanju korisnika nije podložno SQLi napadu jer se pretražuje po id korisnika koji je tipa Integer.</t>
+  </si>
+  <si>
+    <t>CSRF</t>
+  </si>
+  <si>
+    <t>SQLi</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Korišećnje debug features u produkciji poput ispisa steka prilikom obrade izuzetka, iako je korisno za developere pri nalaženju problema, potencijalno daje dosta informacija napadačima o sistemu i njegovim korisnicima i nije bezbedno.</t>
+  </si>
+  <si>
+    <t>CommentRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>GiftRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>HashedUserRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>PermissionRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>PersonRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>RatingRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>RoleRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>TagRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>UserRepositoryEx.png</t>
+  </si>
+  <si>
+    <t>CommentRepositoryEx2.png</t>
+  </si>
+  <si>
+    <t>GiftRepositoryEx2.png</t>
+  </si>
+  <si>
+    <t>HashedUserRepositoryEx2.png</t>
+  </si>
+  <si>
+    <t>PersonRepositoryEx2.png</t>
+  </si>
+  <si>
+    <t>RatingRepositoryEx2.png</t>
+  </si>
+  <si>
+    <t>UserRepositoryEx2.png</t>
+  </si>
+  <si>
+    <t>GiftRepositoryEx3.png</t>
+  </si>
+  <si>
+    <t>GiftRepositoryEx4.png</t>
+  </si>
+  <si>
+    <t>GiftRepositoryEx5.png</t>
+  </si>
+  <si>
+    <t>PersonRepositoryEx3.png</t>
+  </si>
+  <si>
+    <t>PersonRepositoryEx4.png</t>
+  </si>
+  <si>
+    <t>UserRepositoryEx3.png</t>
   </si>
 </sst>
 </file>
@@ -1968,7 +2046,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2154,6 +2232,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2315,7 +2399,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2339,7 +2423,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2390,10 +2475,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
@@ -3633,11 +3718,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="hotspots" displayName="hotspots" ref="A1:L44" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="hotspots" displayName="hotspots" ref="A1:L44" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:L44" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Rule"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Message" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Message" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Category"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Priority"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Severity"/>
@@ -3654,7 +3739,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="metrics" displayName="metrics" ref="A1:I50" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="metrics" displayName="metrics" ref="A1:I50" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:I50" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Path"/>
@@ -9892,10 +9977,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9907,9 +9992,12 @@
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
     <col min="12" max="12" width="29.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9946,8 +10034,17 @@
       <c r="L1" s="2" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>602</v>
+      </c>
+      <c r="O1" t="s">
+        <v>558</v>
+      </c>
+      <c r="P1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>373</v>
       </c>
@@ -9984,8 +10081,17 @@
       <c r="L2" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>599</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>379</v>
       </c>
@@ -10022,8 +10128,17 @@
       <c r="L3" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>600</v>
+      </c>
+      <c r="O3">
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>379</v>
       </c>
@@ -10051,7 +10166,7 @@
       <c r="I4" t="s">
         <v>378</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K4" t="s">
@@ -10060,8 +10175,17 @@
       <c r="L4" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>601</v>
+      </c>
+      <c r="O4">
+        <v>21</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>379</v>
       </c>
@@ -10099,7 +10223,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>379</v>
       </c>
@@ -10127,7 +10251,7 @@
       <c r="I6" t="s">
         <v>378</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K6" t="s">
@@ -10137,7 +10261,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>379</v>
       </c>
@@ -10165,7 +10289,7 @@
       <c r="I7" t="s">
         <v>378</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K7" t="s">
@@ -10175,7 +10299,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>379</v>
       </c>
@@ -10203,7 +10327,7 @@
       <c r="I8" t="s">
         <v>378</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K8" t="s">
@@ -10213,7 +10337,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>379</v>
       </c>
@@ -10241,7 +10365,7 @@
       <c r="I9" t="s">
         <v>378</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K9" t="s">
@@ -10251,7 +10375,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>379</v>
       </c>
@@ -10279,7 +10403,7 @@
       <c r="I10" t="s">
         <v>378</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K10" t="s">
@@ -10289,7 +10413,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>379</v>
       </c>
@@ -10317,7 +10441,7 @@
       <c r="I11" t="s">
         <v>378</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K11" t="s">
@@ -10327,7 +10451,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>379</v>
       </c>
@@ -10365,7 +10489,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>379</v>
       </c>
@@ -10393,7 +10517,7 @@
       <c r="I13" t="s">
         <v>378</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K13" t="s">
@@ -10403,7 +10527,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>379</v>
       </c>
@@ -10441,7 +10565,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>379</v>
       </c>
@@ -10469,7 +10593,7 @@
       <c r="I15" t="s">
         <v>378</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K15" t="s">
@@ -10479,7 +10603,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>379</v>
       </c>
@@ -10507,7 +10631,7 @@
       <c r="I16" t="s">
         <v>378</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K16" t="s">
@@ -10583,7 +10707,7 @@
       <c r="I18" t="s">
         <v>378</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K18" t="s">
@@ -10621,7 +10745,7 @@
       <c r="I19" t="s">
         <v>378</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K19" t="s">
@@ -10659,7 +10783,7 @@
       <c r="I20" t="s">
         <v>378</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K20" t="s">
@@ -10773,7 +10897,7 @@
       <c r="I23" t="s">
         <v>378</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="12" t="s">
         <v>562</v>
       </c>
       <c r="K23" t="s">
@@ -10811,11 +10935,14 @@
       <c r="I24" t="s">
         <v>378</v>
       </c>
-      <c r="J24" t="s">
-        <v>23</v>
+      <c r="J24" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K24" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L24" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -10846,11 +10973,14 @@
       <c r="I25" t="s">
         <v>378</v>
       </c>
-      <c r="J25" t="s">
-        <v>23</v>
+      <c r="J25" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K25" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L25" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -10881,11 +11011,14 @@
       <c r="I26" t="s">
         <v>378</v>
       </c>
-      <c r="J26" t="s">
-        <v>23</v>
+      <c r="J26" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K26" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L26" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -10916,11 +11049,14 @@
       <c r="I27" t="s">
         <v>378</v>
       </c>
-      <c r="J27" t="s">
-        <v>23</v>
+      <c r="J27" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K27" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L27" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -10951,11 +11087,14 @@
       <c r="I28" t="s">
         <v>378</v>
       </c>
-      <c r="J28" t="s">
-        <v>23</v>
+      <c r="J28" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K28" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L28" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -10986,11 +11125,14 @@
       <c r="I29" t="s">
         <v>378</v>
       </c>
-      <c r="J29" t="s">
-        <v>23</v>
+      <c r="J29" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K29" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L29" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -11021,11 +11163,14 @@
       <c r="I30" t="s">
         <v>378</v>
       </c>
-      <c r="J30" t="s">
-        <v>23</v>
+      <c r="J30" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K30" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L30" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -11056,11 +11201,14 @@
       <c r="I31" t="s">
         <v>378</v>
       </c>
-      <c r="J31" t="s">
-        <v>23</v>
+      <c r="J31" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K31" t="s">
-        <v>23</v>
+        <v>603</v>
+      </c>
+      <c r="L31" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -11091,14 +11239,17 @@
       <c r="I32" t="s">
         <v>378</v>
       </c>
-      <c r="J32" t="s">
-        <v>23</v>
+      <c r="J32" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L32" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>398</v>
       </c>
@@ -11126,14 +11277,17 @@
       <c r="I33" t="s">
         <v>378</v>
       </c>
-      <c r="J33" t="s">
-        <v>23</v>
+      <c r="J33" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L33" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>398</v>
       </c>
@@ -11161,14 +11315,17 @@
       <c r="I34" t="s">
         <v>378</v>
       </c>
-      <c r="J34" t="s">
-        <v>23</v>
+      <c r="J34" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L34" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>398</v>
       </c>
@@ -11196,14 +11353,17 @@
       <c r="I35" t="s">
         <v>378</v>
       </c>
-      <c r="J35" t="s">
-        <v>23</v>
+      <c r="J35" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L35" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>398</v>
       </c>
@@ -11231,14 +11391,17 @@
       <c r="I36" t="s">
         <v>378</v>
       </c>
-      <c r="J36" t="s">
-        <v>23</v>
+      <c r="J36" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L36" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>398</v>
       </c>
@@ -11266,14 +11429,17 @@
       <c r="I37" t="s">
         <v>378</v>
       </c>
-      <c r="J37" t="s">
-        <v>23</v>
+      <c r="J37" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L37" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -11301,14 +11467,17 @@
       <c r="I38" t="s">
         <v>378</v>
       </c>
-      <c r="J38" t="s">
-        <v>23</v>
+      <c r="J38" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L38" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>398</v>
       </c>
@@ -11336,14 +11505,17 @@
       <c r="I39" t="s">
         <v>378</v>
       </c>
-      <c r="J39" t="s">
-        <v>23</v>
+      <c r="J39" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L39" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>398</v>
       </c>
@@ -11371,14 +11543,17 @@
       <c r="I40" t="s">
         <v>378</v>
       </c>
-      <c r="J40" t="s">
-        <v>23</v>
+      <c r="J40" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L40" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>398</v>
       </c>
@@ -11406,14 +11581,17 @@
       <c r="I41" t="s">
         <v>378</v>
       </c>
-      <c r="J41" t="s">
-        <v>23</v>
+      <c r="J41" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L41" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>398</v>
       </c>
@@ -11441,14 +11619,17 @@
       <c r="I42" t="s">
         <v>378</v>
       </c>
-      <c r="J42" t="s">
-        <v>23</v>
+      <c r="J42" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L42" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>398</v>
       </c>
@@ -11476,14 +11657,17 @@
       <c r="I43" t="s">
         <v>378</v>
       </c>
-      <c r="J43" t="s">
-        <v>23</v>
+      <c r="J43" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L43" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>398</v>
       </c>
@@ -11511,12 +11695,18 @@
       <c r="I44" t="s">
         <v>378</v>
       </c>
-      <c r="J44" t="s">
-        <v>23</v>
+      <c r="J44" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="K44" t="s">
-        <v>23</v>
-      </c>
+        <v>603</v>
+      </c>
+      <c r="L44" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J45" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>